<commit_message>
in Agregate Codes Hours add merging only those hours which are in current month #5
</commit_message>
<xml_diff>
--- a/Luxoft_Timesheet_27_2017_Denys_LebedevV70.xlsx
+++ b/Luxoft_Timesheet_27_2017_Denys_LebedevV70.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergii\PycharmProjects\Summary_report_renamer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8070" tabRatio="304"/>
   </bookViews>
@@ -13,9 +18,9 @@
   </sheets>
   <definedNames>
     <definedName name="_filter2" localSheetId="1">'List data'!$A$1:$B$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'List data'!$A$1:$B$24</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">'List data'!$A$1:$B$24</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="1">'List data'!$A$1:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'List data'!$A$1:$B$24</definedName>
     <definedName name="Range1">OFFSET('List data'!$A$2,MATCH("*"&amp;Timesheet!#REF!&amp;"*",'List data'!$A$2:$A$54,0)-1,0,COUNTA('List data'!$A:$A))</definedName>
     <definedName name="Range10">OFFSET('List data'!$A$2,MATCH("*"&amp;Timesheet!$A$12&amp;"*",'List data'!$A$2:$A$54,0)-1,0,COUNTA('List data'!$A:$A))</definedName>
     <definedName name="Range11">OFFSET('List data'!$A$2,MATCH("*"&amp;Timesheet!$A$13&amp;"*",'List data'!$A$2:$A$54,0)-1,0,COUNTA('List data'!$A:$A))</definedName>
@@ -37,12 +42,12 @@
     <definedName name="Range8">OFFSET('List data'!$A$2,MATCH("*"&amp;Timesheet!$A$10&amp;"*",'List data'!$A$2:$A$54,0)-1,0,COUNTA('List data'!$A:$A))</definedName>
     <definedName name="Range9">OFFSET('List data'!$A$2,MATCH("*"&amp;Timesheet!$A$11&amp;"*",'List data'!$A$2:$A$54,0)-1,0,COUNTA('List data'!$A:$A))</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="155">
   <si>
     <t>Week</t>
   </si>
@@ -604,6 +609,9 @@
   </si>
   <si>
     <t>Test execution, including environment setup and bug reporting</t>
+  </si>
+  <si>
+    <t>tt</t>
   </si>
 </sst>
 </file>
@@ -1833,56 +1841,37 @@
     </xf>
   </cellXfs>
   <cellStyles count="64">
-    <cellStyle name="20% - Accent1" xfId="23" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="51"/>
-    <cellStyle name="20% - Accent2" xfId="27" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent2 2" xfId="53"/>
-    <cellStyle name="20% - Accent3" xfId="31" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Accent3 2" xfId="55"/>
-    <cellStyle name="20% - Accent4" xfId="35" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Accent4 2" xfId="57"/>
-    <cellStyle name="20% - Accent5" xfId="39" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Accent5 2" xfId="59"/>
-    <cellStyle name="20% - Accent6" xfId="43" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20% - Accent6 2" xfId="61"/>
-    <cellStyle name="40% - Accent1" xfId="24" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="23" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="27" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="31" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="35" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="39" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="43" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40% - Accent1 2" xfId="52"/>
-    <cellStyle name="40% - Accent2" xfId="28" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Accent2 2" xfId="54"/>
-    <cellStyle name="40% - Accent3" xfId="32" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Accent3 2" xfId="56"/>
-    <cellStyle name="40% - Accent4" xfId="36" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent4 2" xfId="58"/>
-    <cellStyle name="40% - Accent5" xfId="40" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent5 2" xfId="60"/>
-    <cellStyle name="40% - Accent6" xfId="44" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40% - Accent6 2" xfId="62"/>
-    <cellStyle name="60% - Accent1" xfId="25" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="29" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="33" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="37" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="41" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="45" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="22" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="26" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="30" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="34" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="38" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="42" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="12" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="24" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="28" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="32" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="36" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="40" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="44" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="25" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="29" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="33" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="37" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="41" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="45" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Currency 2" xfId="63"/>
-    <cellStyle name="Explanatory Text" xfId="20" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="11" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="7" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="9" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="10" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="14" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="17" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="13" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="5"/>
     <cellStyle name="Normal 2 3" xfId="48"/>
@@ -1891,12 +1880,31 @@
     <cellStyle name="Normal 4" xfId="46"/>
     <cellStyle name="Note 2" xfId="50"/>
     <cellStyle name="Note 3" xfId="47"/>
-    <cellStyle name="Output" xfId="15" builtinId="21" customBuiltin="1"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
     <cellStyle name="TableStyleLight1 2" xfId="4"/>
-    <cellStyle name="Title" xfId="6" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="21" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="19" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="22" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="26" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="30" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="34" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="38" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="42" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="14" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="15" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Заголовок 1" xfId="7" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="8" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="9" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="10" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="21" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="6" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="13" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="12" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="20" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="17" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="19" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="11" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1980,9 +1988,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2020,9 +2028,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2057,7 +2065,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2092,7 +2100,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2266,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,29 +2296,29 @@
         <v>0</v>
       </c>
       <c r="C1" s="2">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2">
         <v>2017</v>
       </c>
       <c r="E1" s="3">
         <f>DATE(D1,1,2)-WEEKDAY(DATE(D1,1,2),3)+7*(C1-1)</f>
-        <v>42919</v>
+        <v>42947</v>
       </c>
       <c r="F1" s="4">
         <f>E1</f>
-        <v>42919</v>
+        <v>42947</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="6">
         <f>E1 + 6</f>
-        <v>42925</v>
+        <v>42953</v>
       </c>
       <c r="I1" s="4">
         <f>E1 + 6</f>
-        <v>42925</v>
+        <v>42953</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -2335,31 +2343,31 @@
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="82">
         <f>DATE(D1,1,2)-WEEKDAY(DATE(D1,1,2),3)+7*(C1-1)</f>
-        <v>42919</v>
+        <v>42947</v>
       </c>
       <c r="F5" s="81">
         <f>E1 + 1</f>
-        <v>42920</v>
+        <v>42948</v>
       </c>
       <c r="G5" s="81">
         <f>E1 + 2</f>
-        <v>42921</v>
+        <v>42949</v>
       </c>
       <c r="H5" s="81">
         <f>E1 + 3</f>
-        <v>42922</v>
+        <v>42950</v>
       </c>
       <c r="I5" s="81">
         <f>E1 + 4</f>
-        <v>42923</v>
+        <v>42951</v>
       </c>
       <c r="J5" s="81">
         <f>E1 + 5</f>
-        <v>42924</v>
+        <v>42952</v>
       </c>
       <c r="K5" s="81">
         <f>E1 + 6</f>
-        <v>42925</v>
+        <v>42953</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>3</v>
@@ -2464,7 +2472,7 @@
       <c r="J8" s="21"/>
       <c r="K8" s="22"/>
       <c r="L8" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R8">
         <f>IF(ISNA(MATCH("*"&amp; A8 &amp;"*",'List data'!$A$2:$A$24,0)+1), MATCH(".*"&amp; A8 &amp;".*",'List data'!$A$2:$A$24,0)+1, MATCH("*"&amp; A8 &amp;"*",'List data'!$A$2:$A$24,0)+1)</f>
@@ -2912,6 +2920,24 @@
         <v>21</v>
       </c>
       <c r="B32" s="41"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>SUM(E7:I8)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="69">
+        <f>SUM(E9:H9)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="69">
+        <f>SUM(E10:H10)</f>
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B7:B21">

</xml_diff>